<commit_message>
saved failed message into file
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA8CFCE0-1DC7-4D8F-B0B6-DDC6C1C20575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43B4BB85-4852-42DE-87D1-FBAF6302A025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,25 +447,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>9110125495</v>
+        <v>8273873833</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>12313213231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>132123123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>132123123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>